<commit_message>
fix AMS test bug
</commit_message>
<xml_diff>
--- a/scoring/tests/AMS/AMSC93_test_1.xlsx
+++ b/scoring/tests/AMS/AMSC93_test_1.xlsx
@@ -792,7 +792,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>23</v>
+        <v>21</v>
       </c>
     </row>
     <row r="7">
@@ -812,7 +812,7 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="9">

</xml_diff>